<commit_message>
updated docs and gantt chart timescales
</commit_message>
<xml_diff>
--- a/docs/GanttChart.xlsx
+++ b/docs/GanttChart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,27 +41,6 @@
     <t>Axis Values</t>
   </si>
   <si>
-    <t>Project Title</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
-    <t>Task 8</t>
-  </si>
-  <si>
     <t>Range for Gantt Chart</t>
   </si>
   <si>
@@ -78,6 +57,27 @@
   </si>
   <si>
     <t xml:space="preserve">Design &amp; Implement Database / Normalise </t>
+  </si>
+  <si>
+    <t>Develop Service Layer</t>
+  </si>
+  <si>
+    <t>Develop Repository Layer</t>
+  </si>
+  <si>
+    <t>Develop nHibernate Mappings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop Controllers </t>
+  </si>
+  <si>
+    <t>Develop Views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site CSS Design </t>
+  </si>
+  <si>
+    <t>TravelMe</t>
   </si>
 </sst>
 </file>
@@ -240,22 +240,22 @@
                   <c:v>Design &amp; Implement Database / Normalise </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Task 3</c:v>
+                  <c:v>Develop Repository Layer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Task 4</c:v>
+                  <c:v>Develop nHibernate Mappings</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 5</c:v>
+                  <c:v>Develop Service Layer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Task 6</c:v>
+                  <c:v>Develop Controllers </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Task 7</c:v>
+                  <c:v>Develop Views</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Task 8</c:v>
+                  <c:v>Site CSS Design </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -273,22 +273,22 @@
                   <c:v>42240.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42247.0</c:v>
+                  <c:v>42243.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42252.0</c:v>
+                  <c:v>42248.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42259.0</c:v>
+                  <c:v>42253.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42273.0</c:v>
+                  <c:v>42260.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42278.0</c:v>
+                  <c:v>42265.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42281.0</c:v>
+                  <c:v>42272.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,22 +369,22 @@
                   <c:v>Design &amp; Implement Database / Normalise </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Task 3</c:v>
+                  <c:v>Develop Repository Layer</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Task 4</c:v>
+                  <c:v>Develop nHibernate Mappings</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 5</c:v>
+                  <c:v>Develop Service Layer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Task 6</c:v>
+                  <c:v>Develop Controllers </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Task 7</c:v>
+                  <c:v>Develop Views</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Task 8</c:v>
+                  <c:v>Site CSS Design </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -399,25 +399,25 @@
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -434,11 +434,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2117681984"/>
-        <c:axId val="-2117674432"/>
+        <c:axId val="-2129650704"/>
+        <c:axId val="-2129654272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2117681984"/>
+        <c:axId val="-2129650704"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -481,7 +481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117674432"/>
+        <c:crossAx val="-2129654272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -489,7 +489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117674432"/>
+        <c:axId val="-2129654272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42287.0"/>
@@ -542,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117681984"/>
+        <c:crossAx val="-2129650704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1462,7 +1462,7 @@
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1473,14 +1473,14 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="H2" s="7"/>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="H3" s="1"/>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6">
         <v>42233</v>
@@ -1526,126 +1526,126 @@
         <v>42233</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <f>E4</f>
         <v>42240</v>
       </c>
       <c r="D5" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E11" si="0">C5+D5</f>
-        <v>42247</v>
+        <v>42243</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="5">
         <f>E11+1</f>
-        <v>42289</v>
+        <v>42287</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ref="C6:C11" si="1">E5</f>
-        <v>42247</v>
+        <v>42243</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>42252</v>
+        <v>42248</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
-        <v>42252</v>
+        <v>42248</v>
       </c>
       <c r="D7" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>42259</v>
+        <v>42253</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
-        <v>42259</v>
+        <v>42253</v>
       </c>
       <c r="D8" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>42273</v>
+        <v>42260</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
-        <v>42273</v>
+        <v>42260</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>42278</v>
+        <v>42265</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
-        <v>42278</v>
+        <v>42265</v>
       </c>
       <c r="D10" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>42281</v>
+        <v>42272</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
-        <v>42281</v>
+        <v>42272</v>
       </c>
       <c r="D11" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>42288</v>
+        <v>42286</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Touched up spec and added task to gantt chart
</commit_message>
<xml_diff>
--- a/docs/GanttChart.xlsx
+++ b/docs/GanttChart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Tasks</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Range for Gantt Chart</t>
   </si>
   <si>
-    <t xml:space="preserve">When changing things, right click on the y axis and format it. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Change the Max and Min to the range table values. </t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t xml:space="preserve">Design &amp; Implement Database / Normalise </t>
   </si>
   <si>
-    <t>Develop Service Layer</t>
-  </si>
-  <si>
     <t>Develop Repository Layer</t>
   </si>
   <si>
@@ -78,6 +72,15 @@
   </si>
   <si>
     <t>TravelMe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When changing things, right click on the y axis and format it.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop Service Layer </t>
+  </si>
+  <si>
+    <t>Site JavaScript Design</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,13 +156,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -170,6 +184,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -210,9 +228,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Start Date</c:v>
-          </c:tx>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -230,9 +245,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Define Requirements, User Stories, Database Objects</c:v>
                 </c:pt>
@@ -246,7 +261,7 @@
                   <c:v>Develop nHibernate Mappings</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Develop Service Layer</c:v>
+                  <c:v>Develop Service Layer </c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Develop Controllers </c:v>
@@ -256,16 +271,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Site CSS Design </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Site JavaScript Design</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$11</c:f>
+              <c:f>Sheet1!$C$4:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>42233.0</c:v>
                 </c:pt>
@@ -289,6 +307,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>42272.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42286.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -297,9 +318,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Duration</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1">
@@ -359,9 +377,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:f>Sheet1!$B$4:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Define Requirements, User Stories, Database Objects</c:v>
                 </c:pt>
@@ -375,7 +393,7 @@
                   <c:v>Develop nHibernate Mappings</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Develop Service Layer</c:v>
+                  <c:v>Develop Service Layer </c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Develop Controllers </c:v>
@@ -385,16 +403,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Site CSS Design </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Site JavaScript Design</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$11</c:f>
+              <c:f>Sheet1!$D$4:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>7.0</c:v>
                 </c:pt>
@@ -417,6 +438,9 @@
                   <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -492,7 +516,7 @@
         <c:axId val="-2129654272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="42287.0"/>
+          <c:max val="42300.0"/>
           <c:min val="42233.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1107,15 +1131,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1459,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J15"/>
+  <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,19 +1495,27 @@
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1496,17 +1528,23 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="J3" t="s">
-        <v>7</v>
-      </c>
+      <c r="G3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6">
         <v>42233</v>
@@ -1518,20 +1556,23 @@
         <f>C4+D4</f>
         <v>42240</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5">
-        <f>C4</f>
-        <v>42233</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <f>E4</f>
@@ -1541,23 +1582,32 @@
         <v>3</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E11" si="0">C5+D5</f>
+        <f t="shared" ref="E5:E12" si="0">C5+D5</f>
         <v>42243</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5">
-        <f>E11+1</f>
-        <v>42287</v>
-      </c>
+        <f>C4</f>
+        <v>42233</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ref="C6:C11" si="1">E5</f>
+        <f t="shared" ref="C6:C12" si="1">E5</f>
         <v>42243</v>
       </c>
       <c r="D6" s="1">
@@ -1567,10 +1617,16 @@
         <f t="shared" si="0"/>
         <v>42248</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>42300</v>
+      </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
@@ -1584,9 +1640,9 @@
         <v>42253</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="1"/>
@@ -1600,9 +1656,9 @@
         <v>42260</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="1"/>
@@ -1616,9 +1672,9 @@
         <v>42265</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
@@ -1632,9 +1688,9 @@
         <v>42272</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
@@ -1648,15 +1704,34 @@
         <v>42286</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="1"/>
+        <v>42286</v>
+      </c>
+      <c r="D12" s="9">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>42300</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G2:H2"/>
+  <mergeCells count="4">
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J2:L5"/>
+    <mergeCell ref="M2:O5"/>
+    <mergeCell ref="P2:R5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>